<commit_message>
to make build stable
</commit_message>
<xml_diff>
--- a/src/main/resources/testData.xlsx
+++ b/src/main/resources/testData.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="22">
   <si>
     <t>Flag</t>
   </si>
@@ -62,6 +62,9 @@
     <t>loginParams</t>
   </si>
   <si>
+    <t>RequestHeaders</t>
+  </si>
+  <si>
     <t>Get Student Photo</t>
   </si>
   <si>
@@ -69,6 +72,9 @@
   </si>
   <si>
     <t>GET</t>
+  </si>
+  <si>
+    <t>defaultHeaders</t>
   </si>
   <si>
     <t>studentPhoto</t>
@@ -1497,7 +1503,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1507,14 +1513,15 @@
     <col min="2" max="2" width="23" style="10" customWidth="1"/>
     <col min="3" max="3" width="15" style="10" customWidth="1"/>
     <col min="4" max="4" width="13.1719" style="10" customWidth="1"/>
-    <col min="5" max="5" width="13.1719" style="10" customWidth="1"/>
-    <col min="6" max="6" width="13.8516" style="10" customWidth="1"/>
+    <col min="5" max="5" width="16" style="10" customWidth="1"/>
+    <col min="6" max="6" width="13.1719" style="10" customWidth="1"/>
     <col min="7" max="7" width="13.8516" style="10" customWidth="1"/>
-    <col min="8" max="8" width="19.1719" style="10" customWidth="1"/>
-    <col min="9" max="9" width="22.3516" style="10" customWidth="1"/>
-    <col min="10" max="10" width="11.1719" style="10" customWidth="1"/>
-    <col min="11" max="11" width="8.67188" style="10" customWidth="1"/>
-    <col min="12" max="256" width="8.85156" style="10" customWidth="1"/>
+    <col min="8" max="8" width="13.8516" style="10" customWidth="1"/>
+    <col min="9" max="9" width="19.1719" style="10" customWidth="1"/>
+    <col min="10" max="10" width="22.3516" style="10" customWidth="1"/>
+    <col min="11" max="11" width="11.1719" style="10" customWidth="1"/>
+    <col min="12" max="12" width="8.67188" style="10" customWidth="1"/>
+    <col min="13" max="256" width="8.85156" style="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="16.6" customHeight="1">
@@ -1531,24 +1538,27 @@
         <v>3</v>
       </c>
       <c r="E1" t="s" s="2">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s" s="2">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="2">
+      <c r="G1" t="s" s="2">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="2">
+      <c r="H1" t="s" s="2">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="2">
+      <c r="I1" t="s" s="2">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="2">
+      <c r="J1" t="s" s="2">
         <v>8</v>
       </c>
-      <c r="J1" t="s" s="2">
+      <c r="K1" t="s" s="2">
         <v>9</v>
       </c>
-      <c r="K1" t="s" s="2">
+      <c r="L1" t="s" s="2">
         <v>10</v>
       </c>
     </row>
@@ -1557,23 +1567,26 @@
         <v>11</v>
       </c>
       <c r="B2" t="s" s="3">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s" s="4">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s" s="3">
-        <v>18</v>
-      </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="3"/>
-      <c r="G2" t="s" s="3">
         <v>19</v>
       </c>
-      <c r="H2" s="6"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="6"/>
+      <c r="E2" t="s" s="3">
+        <v>20</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="3"/>
+      <c r="H2" t="s" s="3">
+        <v>21</v>
+      </c>
+      <c r="I2" s="6"/>
+      <c r="J2" s="5"/>
       <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
     </row>
     <row r="3" ht="17" customHeight="1">
       <c r="A3" s="5"/>
@@ -1587,6 +1600,7 @@
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
       <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
     </row>
     <row r="4" ht="17" customHeight="1">
       <c r="A4" s="5"/>
@@ -1600,6 +1614,7 @@
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
       <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
     </row>
     <row r="5" ht="17" customHeight="1">
       <c r="A5" s="5"/>
@@ -1613,6 +1628,7 @@
       <c r="I5" s="5"/>
       <c r="J5" s="5"/>
       <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
     </row>
     <row r="6" ht="17" customHeight="1">
       <c r="A6" s="5"/>
@@ -1626,6 +1642,7 @@
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
       <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
     </row>
     <row r="7" ht="17" customHeight="1">
       <c r="A7" s="5"/>
@@ -1639,6 +1656,7 @@
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
       <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
     </row>
     <row r="8" ht="17" customHeight="1">
       <c r="A8" s="5"/>
@@ -1652,6 +1670,7 @@
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
     </row>
     <row r="9" ht="17" customHeight="1">
       <c r="A9" s="5"/>
@@ -1665,6 +1684,21 @@
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
       <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+    </row>
+    <row r="10" ht="17" customHeight="1">
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7875" right="0.7875" top="1.05278" bottom="1.05278" header="0.7875" footer="0.7875"/>

</xml_diff>